<commit_message>
praca magisterska korekta rozdziału 5 21.03.2020
</commit_message>
<xml_diff>
--- a/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
+++ b/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnaKułacz\studia\Magisterka\Praca Magisterska\ImmunochemioTherapyModel\Sprawozdanie\moje\rysunki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9BB5ECA-399F-4950-9817-9D2BB51F96BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01FD6B2-7D4D-402F-84DF-0E2B344F7ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1DC66E2F-FA51-41BE-990C-40A94CDDCB53}"/>
   </bookViews>
@@ -117,13 +117,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -131,17 +137,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Liczba komórek nowotworowych w chwili t = 120 dni</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> - T(120)</a:t>
+              <a:t>Liczba komórek nowotworowych w chwili T = 120 dni - T(120)</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:rPr lang="pl-PL"/>
             </a:br>
             <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:rPr lang="pl-PL"/>
               <a:t>w zależności od początkowej liczby komórek nowotworowych T(0)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
@@ -161,13 +163,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -198,13 +206,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -295,7 +309,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -309,7 +322,9 @@
       <c:valAx>
         <c:axId val="417685728"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="900000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -317,9 +332,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -334,11 +349,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -348,7 +362,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>T(0) [liczbakomórek]</a:t>
+                  <a:t>T(0) [liczba komórek]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -366,11 +380,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -390,25 +403,22 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -426,6 +436,7 @@
       <c:valAx>
         <c:axId val="417685072"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -434,9 +445,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -451,11 +462,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -483,11 +493,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -499,7 +508,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -507,12 +516,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -523,9 +530,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -537,7 +543,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="417685728"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -560,17 +566,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -613,13 +630,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -627,11 +650,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Liczba komórek nowotworowych w chwili t = 120 dni - T(120) </a:t>
+              <a:t>Liczba komórek nowotworowych w chwili T = 120 dni - T(120) </a:t>
             </a:r>
-            <a:br>
-              <a:rPr lang="pl-PL"/>
-            </a:br>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
               <a:t>w zależności od początkowej liczby krążących limfocytów C(0)</a:t>
@@ -652,13 +677,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -689,13 +720,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -807,9 +844,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -824,11 +861,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -843,6 +879,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.43672996219589827"/>
+              <c:y val="0.93578304065963791"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -856,11 +900,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -880,12 +923,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -896,9 +937,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -924,9 +964,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -941,11 +981,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -955,13 +994,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>T(120)</a:t>
+                  <a:t>T(120) [liczba komórek]</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
-                  <a:t> [liczba komórek]</a:t>
-                </a:r>
-                <a:endParaRPr lang="pl-PL"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -978,11 +1012,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1002,12 +1035,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1018,9 +1049,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1055,17 +1085,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1168,62 +1209,66 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1232,9 +1277,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1253,14 +1297,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1269,20 +1305,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1291,13 +1327,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1309,30 +1345,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1348,21 +1385,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1381,14 +1415,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1400,14 +1433,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1421,9 +1454,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1437,12 +1469,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1454,9 +1480,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1471,14 +1497,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1490,14 +1515,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1509,14 +1534,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1525,14 +1549,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1540,7 +1563,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1553,11 +1576,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1565,14 +1596,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1584,12 +1615,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1605,7 +1643,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1614,9 +1652,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1632,14 +1669,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1648,20 +1684,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1673,73 +1706,71 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1748,9 +1779,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1769,14 +1799,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1785,20 +1807,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1807,13 +1829,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1825,30 +1847,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1864,21 +1887,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1897,14 +1917,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1916,14 +1935,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1937,9 +1956,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1953,12 +1971,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1970,9 +1982,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1987,14 +1999,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2006,14 +2017,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2025,14 +2036,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2041,14 +2051,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2056,7 +2065,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2069,11 +2078,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2081,14 +2098,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2100,12 +2117,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2121,7 +2145,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2130,9 +2154,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2148,14 +2171,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2164,20 +2186,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2189,12 +2208,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2204,15 +2217,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>15870</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>15874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2239,16 +2252,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>361955</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>9523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>54030</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>98641</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2575,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E200FD-59F7-4853-9838-C34C44D44042}">
   <dimension ref="D4:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
praca magisterska korekta rozdziału 5 25.03.2020
</commit_message>
<xml_diff>
--- a/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
+++ b/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnaKułacz\studia\Magisterka\Praca Magisterska\ImmunochemioTherapyModel\Sprawozdanie\moje\rysunki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01FD6B2-7D4D-402F-84DF-0E2B344F7ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B90E3D5-7FB9-47C3-AE15-C05F2FD42881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1DC66E2F-FA51-41BE-990C-40A94CDDCB53}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>T(0)</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>C(0)</t>
+  </si>
+  <si>
+    <t>Promień nowotworu</t>
   </si>
 </sst>
 </file>
@@ -117,19 +120,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -163,19 +160,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -206,19 +197,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="15875" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -332,9 +317,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -349,10 +334,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -380,10 +366,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -395,30 +382,33 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -445,9 +435,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -462,10 +452,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -493,10 +484,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -516,10 +508,12 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -530,8 +524,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -566,28 +561,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -659,7 +643,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>w zależności od początkowej liczby krążących limfocytów C(0)</a:t>
+              <a:t>w zależności od początkowej liczby limfocytów </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>krążących</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> C(0)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1128,6 +1122,1025 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Długość promienia nowotworu w chwili T = 120 dni - T(120)</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>w zależności od początkowej liczby komórek nowotworowych T(0)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1245666689295192"/>
+          <c:y val="1.5629358580969102E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Promień nowotworu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$34:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$34:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D802-4B78-9EF9-549F9D285B2B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="428872048"/>
+        <c:axId val="428869424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="428872048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>T(0) [liczba komórek]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44773266124420225"/>
+              <c:y val="0.92918498877629907"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="428869424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="428869424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Promień nowotworu [mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="428872048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Długość promienia nowotworu w chwili T = 120 dni - T(120)</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>w zależności od początkowej liczby limfocytów krążących C(0)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Promień nowotworu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$46:$D$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60000000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3500000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$46:$E$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3124-42FD-A645-ECE2E497A183}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="420572504"/>
+        <c:axId val="420573488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="420572504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>C(0)</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> [liczba komórek]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420573488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="420573488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Promień nowotworu [mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420572504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1208,7 +2221,603 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1710,67 +3319,63 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1779,8 +3384,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1799,6 +3405,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1807,20 +3421,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1829,13 +3443,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1847,31 +3461,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1887,18 +3500,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1917,13 +3533,14 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1935,14 +3552,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1956,8 +3573,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1971,6 +3589,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1982,9 +3606,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1999,13 +3623,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2017,14 +3642,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2036,13 +3661,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2051,13 +3677,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2065,7 +3692,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2078,19 +3705,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2098,14 +3717,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2117,19 +3736,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2145,7 +3757,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2154,8 +3766,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2171,13 +3784,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2186,17 +3800,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2208,6 +3825,528 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2225,7 +4364,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>128814</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2259,9 +4398,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>54030</xdr:colOff>
+      <xdr:colOff>37800</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>98641</xdr:rowOff>
+      <xdr:rowOff>121423</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2281,6 +4420,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>27212</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>145595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>105834</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>68035</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF71E4B-E31E-4131-9309-19C91C28E584}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>105836</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>26174</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{349718E8-6F30-4F01-891D-DCC2703F7BDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2586,10 +4797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E200FD-59F7-4853-9838-C34C44D44042}">
-  <dimension ref="D4:E26"/>
+  <dimension ref="D4:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U58" sqref="U58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,6 +4981,182 @@
         <v>980000000</v>
       </c>
     </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2.6999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1.9000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="1">
+        <v>15000000</v>
+      </c>
+      <c r="E38" s="1">
+        <v>2.1999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1">
+        <v>17000000</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1.9000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1">
+        <v>17500000</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2.0999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1">
+        <v>18000000</v>
+      </c>
+      <c r="E41" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1">
+        <v>20000000</v>
+      </c>
+      <c r="E42" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1">
+        <v>50000000</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1">
+        <v>60000000000</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="1">
+        <v>30000000000</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3.4E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="1">
+        <v>10000000000</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1.5E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1">
+        <v>6000000000</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2.3E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1">
+        <v>4000000000</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2.4000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="1">
+        <v>3500000000</v>
+      </c>
+      <c r="E51" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1">
+        <v>3000000000</v>
+      </c>
+      <c r="E52" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="E53" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="1">
+        <v>600000000</v>
+      </c>
+      <c r="E54" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="1">
+        <v>300000000</v>
+      </c>
+      <c r="E55" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
praca magisterska korekta rozdziału 5 28.03.2020
</commit_message>
<xml_diff>
--- a/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
+++ b/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnaKułacz\studia\Magisterka\Praca Magisterska\ImmunochemioTherapyModel\Sprawozdanie\moje\rysunki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B90E3D5-7FB9-47C3-AE15-C05F2FD42881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51681A39-3C3B-4E34-8860-6E902E6DAAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1DC66E2F-FA51-41BE-990C-40A94CDDCB53}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1DC66E2F-FA51-41BE-990C-40A94CDDCB53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,11 +120,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -134,7 +133,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Liczba komórek nowotworowych w chwili T = 120 dni - T(120)</a:t>
+              <a:t>Liczba komórek nowotworu T(120) w ostatnim</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> dniu symulacji trwającej</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> 120 dni</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="pl-PL"/>
@@ -160,11 +167,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -197,13 +203,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -307,7 +319,6 @@
       <c:valAx>
         <c:axId val="417685728"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
           <c:min val="900000"/>
         </c:scaling>
@@ -317,9 +328,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -334,11 +346,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -347,12 +358,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>T(0) [liczba komórek]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t>Początkowa liczba komórek nowotworowych T(0)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.313650852160477"/>
+              <c:y val="0.93318449206635712"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -366,11 +385,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -390,9 +408,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -400,15 +417,14 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -426,7 +442,6 @@
       <c:valAx>
         <c:axId val="417685072"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -435,9 +450,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -452,11 +468,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -465,8 +480,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>T(120) [liczba komórek]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Liczba komórek nowotworowych po symulacji T(120)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -484,11 +499,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -508,9 +522,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -524,9 +537,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -562,11 +574,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -614,19 +629,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -634,7 +642,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Liczba komórek nowotworowych w chwili T = 120 dni - T(120) </a:t>
+              <a:t>Liczba komórek nowotworu</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> T(120) w ostatnim dniu symulacji trwającej</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> 120 dni </a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -643,17 +659,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>w zależności od początkowej liczby limfocytów </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>krążących</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t> C(0)</a:t>
+              <a:t>w zależności od początkowej liczby limfocytów krążących C(0)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -671,19 +677,12 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -714,18 +713,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="15875" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
             </a:effectLst>
           </c:spPr>
           <c:marker>
@@ -838,9 +837,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -855,7 +855,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -867,8 +867,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>C(0) [liczba komórek]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Początkowa Liczba limfocytów krążących C(0)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -877,8 +877,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.43672996219589827"/>
-              <c:y val="0.93578304065963791"/>
+              <c:x val="0.33246069065034584"/>
+              <c:y val="0.9435994173641884"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -894,7 +894,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -921,6 +921,7 @@
                 <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -958,9 +959,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -975,7 +977,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -987,8 +989,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>T(120) [liczba komórek]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Liczba komórek nowotworowych po symulacji T(120)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1006,7 +1008,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -1033,6 +1035,7 @@
                 <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1079,28 +1082,20 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1143,11 +1138,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1156,25 +1150,16 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Długość promienia nowotworu w chwili T = 120 dni - T(120)</a:t>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Długość promienia nowotworu w ostatnim dniu symulacji trwającej 120 dni</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="pl-PL"/>
             </a:br>
             <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="pl-PL"/>
               <a:t>w zależności od początkowej liczby komórek nowotworowych T(0)</a:t>
             </a:r>
-            <a:endParaRPr lang="pl-PL">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1182,8 +1167,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1245666689295192"/>
-          <c:y val="1.5629358580969102E-2"/>
+          <c:x val="0.18228763196779343"/>
+          <c:y val="2.0839144774625468E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1199,11 +1184,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1236,13 +1220,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1354,9 +1344,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1371,11 +1362,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1384,8 +1374,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>T(0) [liczba komórek]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Początkowa liczba komórek nowotworowych T(0)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1394,8 +1384,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.44773266124420225"/>
-              <c:y val="0.92918498877629907"/>
+              <c:x val="0.34662294757445899"/>
+              <c:y val="0.93439484436276521"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1411,11 +1401,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1435,9 +1424,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1445,15 +1433,14 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="0"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1479,9 +1466,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1496,11 +1484,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1509,8 +1496,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>Promień nowotworu [mm]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Promień nowotworu po symulacji [mm]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1528,11 +1515,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1552,9 +1538,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1568,9 +1553,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1606,11 +1590,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1658,11 +1645,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1671,25 +1657,24 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Długość promienia nowotworu w chwili T = 120 dni - T(120)</a:t>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Długość promienia nowotworu w ostatnim</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> dniu symulacji trwającej</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> 120 dni</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="pl-PL"/>
             </a:br>
             <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="pl-PL"/>
               <a:t>w zależności od początkowej liczby limfocytów krążących C(0)</a:t>
             </a:r>
-            <a:endParaRPr lang="pl-PL">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1706,11 +1691,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1743,13 +1727,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1861,9 +1851,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1878,11 +1869,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1891,14 +1881,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>C(0)</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Początkowa liczba limfocytów krążących C(0)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
-                  <a:t> [liczba komórek]</a:t>
-                </a:r>
-                <a:endParaRPr lang="pl-PL"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1915,11 +1900,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1931,17 +1915,16 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1955,9 +1938,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1983,9 +1965,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2000,11 +1983,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -2013,8 +1995,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>Promień nowotworu [mm]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Promień nowotworu po symulacji [mm]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2032,11 +2014,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2056,9 +2037,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2072,9 +2052,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2110,11 +2089,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -2302,211 +2284,35 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2517,78 +2323,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2596,230 +2331,9 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
-  <cs:axisTitle>
+  </cs:chartArea>
+  <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2828,68 +2342,6 @@
         <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
@@ -2897,14 +2349,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2913,72 +2368,131 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:effectRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3001,9 +2515,9 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3015,22 +2529,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3039,17 +2553,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -3058,13 +2571,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3076,7 +2589,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -3089,9 +2602,10 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3106,13 +2620,15 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3121,17 +2637,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -3140,16 +2655,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3169,7 +2684,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -3177,7 +2692,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3189,15 +2704,6 @@
         <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3205,14 +2711,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3225,18 +2730,10 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3245,14 +2742,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3272,19 +2770,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3304,227 +2804,53 @@
             <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3535,78 +2861,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -3614,295 +2869,15 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3912,23 +2887,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -3936,63 +2906,123 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:effectRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -4016,21 +3046,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4040,7 +3067,328 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4051,16 +3399,296 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -4070,80 +3698,10 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+            <a:alpha val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4155,14 +3713,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4174,14 +3731,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4193,27 +3749,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4221,9 +3776,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4233,14 +3787,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4252,12 +3805,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4266,14 +3818,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4282,9 +3835,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4294,17 +3846,556 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4316,37 +4407,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4356,14 +4440,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>15870</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:colOff>7932</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>15874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:colOff>103187</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>128814</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4391,16 +4475,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>136885</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>22254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>37800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>121423</xdr:rowOff>
+      <xdr:colOff>222310</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>134154</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4428,15 +4512,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>27212</xdr:colOff>
+      <xdr:colOff>90712</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>145595</xdr:rowOff>
+      <xdr:rowOff>113845</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>105834</xdr:colOff>
+      <xdr:colOff>169334</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>68035</xdr:rowOff>
+      <xdr:rowOff>36285</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4464,15 +4548,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
+      <xdr:colOff>215300</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:rowOff>140727</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>105836</xdr:colOff>
+      <xdr:colOff>261724</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>26174</xdr:rowOff>
+      <xdr:rowOff>59444</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4799,8 +4883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E200FD-59F7-4853-9838-C34C44D44042}">
   <dimension ref="D4:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U58" sqref="U58"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AL35" sqref="AL34:AL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
praca magisterska korekta rozdziału 5 30.03.2020
</commit_message>
<xml_diff>
--- a/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
+++ b/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnaKułacz\studia\Magisterka\Praca Magisterska\ImmunochemioTherapyModel\Sprawozdanie\moje\rysunki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51681A39-3C3B-4E34-8860-6E902E6DAAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDB6C6C-36AD-4FB1-9A56-1A6943201425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1DC66E2F-FA51-41BE-990C-40A94CDDCB53}"/>
   </bookViews>
@@ -79,9 +79,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,7 +225,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$5:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000000</c:v>
@@ -263,7 +264,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$5:$E$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.7599999999999997E-8</c:v>
@@ -400,7 +401,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -438,6 +439,70 @@
         <c:crossAx val="417685072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="tenMillions"/>
+          <c:dispUnitsLbl>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000"/>
+                    <a:t>x</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:t> 10</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" strike="noStrike" baseline="30000"/>
+                    <a:t>7</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1000"/>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="417685072"/>
@@ -514,7 +579,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -552,6 +617,66 @@
         <c:crossAx val="417685728"/>
         <c:crossesAt val="0.5"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:custUnit val="1000000000"/>
+          <c:dispUnitsLbl>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:t>x 10</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:t>9</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1000"/>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -734,7 +859,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$17:$D$26</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>60000000000</c:v>
@@ -773,7 +898,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$17:$E$26</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.7599999999999997E-8</c:v>
@@ -909,7 +1034,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -947,6 +1072,66 @@
         <c:crossAx val="590061936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:custUnit val="10000000000"/>
+          <c:dispUnitsLbl>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:t>x 10</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:t>10</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1000"/>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="590061936"/>
@@ -1023,7 +1208,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1061,6 +1246,66 @@
         <c:crossAx val="590061608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:custUnit val="1000000000"/>
+          <c:dispUnitsLbl>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:t>x 10</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:t>9</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1000"/>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1241,7 +1486,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$34:$D$43</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000000</c:v>
@@ -1270,7 +1515,7 @@
                 <c:pt idx="8">
                   <c:v>20000000</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="9" formatCode="0.00E+00">
                   <c:v>50000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -1280,7 +1525,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$34:$E$43</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.5000000000000001E-5</c:v>
@@ -1309,7 +1554,7 @@
                 <c:pt idx="8">
                   <c:v>6.16</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="9" formatCode="0.00E+00">
                   <c:v>6.16</c:v>
                 </c:pt>
               </c:numCache>
@@ -1416,7 +1661,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -1454,6 +1699,66 @@
         <c:crossAx val="428869424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="tenMillions"/>
+          <c:dispUnitsLbl>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:t>x 10</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:t>7</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1000"/>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="428869424"/>
@@ -1530,7 +1835,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1748,7 +2053,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$46:$D$55</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>60000000000</c:v>
@@ -1787,7 +2092,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$46:$E$55</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.5000000000000001E-5</c:v>
@@ -1915,7 +2220,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -1953,6 +2258,65 @@
         <c:crossAx val="420573488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:custUnit val="10000000000"/>
+          <c:dispUnitsLbl>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:t>x 10</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:t>10</a:t>
+                  </a:r>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="420573488"/>
@@ -2029,7 +2393,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4883,11 +5247,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E200FD-59F7-4853-9838-C34C44D44042}">
   <dimension ref="D4:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AL35" sqref="AL34:AL35"/>
+    <sheetView tabSelected="1" topLeftCell="P31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
@@ -4898,82 +5266,82 @@
       </c>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>1000000</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>6.7599999999999997E-8</v>
       </c>
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>2000000</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>8.1499999999999995E-8</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>5000000</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>2.6899999999999999E-8</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>10000000</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>3.4399999999999997E-8</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>15000000</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>4.4099999999999998E-8</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>17000000</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>2.96E-8</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>17500000</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>3.6699999999999998E-8</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>18000000</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>980000000</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>20000000</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>980000000</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>50000000</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>980000000</v>
       </c>
     </row>
@@ -4986,82 +5354,82 @@
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <v>60000000000</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>6.7599999999999997E-8</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>30000000000</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <v>1.6899999999999999E-7</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="1">
+      <c r="D19" s="2">
         <v>10000000000</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
         <v>3.0899999999999999E-8</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="1">
+      <c r="D20" s="2">
         <v>6000000000</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="2">
         <v>4.7899999999999999E-8</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <v>4000000000</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="2">
         <v>5.7200000000000003E-8</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>3500000000</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="2">
         <v>980000000</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="1">
+      <c r="D23" s="2">
         <v>3000000000</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="2">
         <v>980000000</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="1">
+      <c r="D24" s="2">
         <v>1000000000</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="2">
         <v>980000000</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="1">
+      <c r="D25" s="2">
         <v>600000000</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="2">
         <v>980000000</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="1">
+      <c r="D26" s="2">
         <v>300000000</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="2">
         <v>980000000</v>
       </c>
     </row>
@@ -5074,74 +5442,74 @@
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="1">
+      <c r="D34" s="2">
         <v>1000000</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="2">
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="1">
+      <c r="D35" s="2">
         <v>2000000</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="2">
         <v>2.6999999999999999E-5</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="1">
+      <c r="D36" s="2">
         <v>5000000</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="2">
         <v>1.9000000000000001E-5</v>
       </c>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D37" s="1">
+      <c r="D37" s="2">
         <v>10000000</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="1">
+      <c r="D38" s="2">
         <v>15000000</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2">
         <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="1">
+      <c r="D39" s="2">
         <v>17000000</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="2">
         <v>1.9000000000000001E-5</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D40" s="1">
+      <c r="D40" s="2">
         <v>17500000</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="2">
         <v>2.0999999999999999E-5</v>
       </c>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D41" s="1">
+      <c r="D41" s="2">
         <v>18000000</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="2">
         <v>6.16</v>
       </c>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D42" s="1">
+      <c r="D42" s="2">
         <v>20000000</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="2">
         <v>6.16</v>
       </c>
     </row>
@@ -5162,82 +5530,82 @@
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D46" s="1">
+      <c r="D46" s="2">
         <v>60000000000</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="2">
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D47" s="1">
+      <c r="D47" s="2">
         <v>30000000000</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="2">
         <v>3.4E-5</v>
       </c>
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D48" s="1">
+      <c r="D48" s="2">
         <v>10000000000</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="2">
         <v>1.5E-5</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D49" s="1">
+      <c r="D49" s="2">
         <v>6000000000</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="2">
         <v>2.3E-5</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D50" s="1">
+      <c r="D50" s="2">
         <v>4000000000</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="2">
         <v>2.4000000000000001E-5</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="1">
+      <c r="D51" s="2">
         <v>3500000000</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="2">
         <v>6.16</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="1">
+      <c r="D52" s="2">
         <v>3000000000</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="2">
         <v>6.16</v>
       </c>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D53" s="1">
+      <c r="D53" s="2">
         <v>1000000000</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="2">
         <v>6.16</v>
       </c>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D54" s="1">
+      <c r="D54" s="2">
         <v>600000000</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="2">
         <v>6.16</v>
       </c>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D55" s="1">
+      <c r="D55" s="2">
         <v>300000000</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="2">
         <v>6.16</v>
       </c>
     </row>

</xml_diff>